<commit_message>
Finished renaming LSI -> LIQ
</commit_message>
<xml_diff>
--- a/data_raw/dicts/LIQ_dict.xlsx
+++ b/data_raw/dicts/LIQ_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D053F2-B49D-409C-9E7B-D3FA7B19D260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E40A5C-59E3-4F3D-B31D-071DC2C4EFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LIQ_dict" sheetId="1" r:id="rId1"/>
@@ -61,24 +61,12 @@
     <t>Sach- und Fachliteratur</t>
   </si>
   <si>
-    <t>TLSI_0000_PROMPT</t>
-  </si>
-  <si>
-    <t>TLSI_0001_PROMPT</t>
-  </si>
-  <si>
     <t>The following questions are about your interest in and engagement with literature.</t>
   </si>
   <si>
     <t xml:space="preserve">What kind(s) of literature do you like best? </t>
   </si>
   <si>
-    <t>TLSI_0002_PROMPT</t>
-  </si>
-  <si>
-    <t>TLSI_0003_PROMPT</t>
-  </si>
-  <si>
     <t>sehr ungern</t>
   </si>
   <si>
@@ -100,42 +88,12 @@
     <t>sehr gern</t>
   </si>
   <si>
-    <t>TLSI_0003_CHOICE1</t>
-  </si>
-  <si>
-    <t>TLSI_0003_CHOICE2</t>
-  </si>
-  <si>
-    <t>TLSI_0003_CHOICE3</t>
-  </si>
-  <si>
-    <t>TLSI_0003_CHOICE4</t>
-  </si>
-  <si>
-    <t>TLSI_0003_CHOICE5</t>
-  </si>
-  <si>
-    <t>TLSI_0003_CHOICE6</t>
-  </si>
-  <si>
-    <t>TLSI_0003_CHOICE7</t>
-  </si>
-  <si>
     <t>neither nor</t>
   </si>
   <si>
     <t>very much</t>
   </si>
   <si>
-    <t>TLSI_0004_PROMPT</t>
-  </si>
-  <si>
-    <t>TLSI_0004_CHOICE1</t>
-  </si>
-  <si>
-    <t>TLSI_0004_CHOICE2</t>
-  </si>
-  <si>
     <t>Ja</t>
   </si>
   <si>
@@ -148,12 +106,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>TLSI_0005_PROMPT</t>
-  </si>
-  <si>
-    <t>TLSI_0005_UNIT</t>
-  </si>
-  <si>
     <t>Stunden</t>
   </si>
   <si>
@@ -175,75 +127,9 @@
     <t>Poetry (all types of poems, poetry)</t>
   </si>
   <si>
-    <t>TLSI_0005_OPTION1</t>
-  </si>
-  <si>
-    <t>TLSI_0005_OPTION2</t>
-  </si>
-  <si>
-    <t>TLSI_0005_OPTION3</t>
-  </si>
-  <si>
-    <t>TLSI_0005_OPTION4</t>
-  </si>
-  <si>
-    <t>TLSI_0005_OPTION5</t>
-  </si>
-  <si>
-    <t>TLSI_0006_PROMPT</t>
-  </si>
-  <si>
-    <t>TLSI_0006_UNIT</t>
-  </si>
-  <si>
-    <t>TLSI_0006_OPTION1</t>
-  </si>
-  <si>
-    <t>TLSI_0006_OPTION2</t>
-  </si>
-  <si>
-    <t>TLSI_0006_OPTION3</t>
-  </si>
-  <si>
-    <t>TLSI_0006_OPTION4</t>
-  </si>
-  <si>
-    <t>TLSI_0006_OPTION5</t>
-  </si>
-  <si>
     <t>Denken Sie nun bitte einmal an die Zeit in Ihrem Leben, als Sie sich am meisten mit Literatur beschäftigt haben. \\ Wie viele Stunden haben Sie auf dem Höhepunkt Ihres literarischen Interesses durchschnittlich in einer Woche damit verbracht, die folgenden literarischen Gattungen zu lesen.</t>
   </si>
   <si>
-    <t>TLSI_0007_PROMPT</t>
-  </si>
-  <si>
-    <t>TLSI_0007_UNIT</t>
-  </si>
-  <si>
-    <t>TLSI_0007_OPTION1</t>
-  </si>
-  <si>
-    <t>TLSI_0007_OPTION2</t>
-  </si>
-  <si>
-    <t>TLSI_0008_PROMPT</t>
-  </si>
-  <si>
-    <t>TLSI_0008_UNIT</t>
-  </si>
-  <si>
-    <t>TLSI_0008_OPTION1</t>
-  </si>
-  <si>
-    <t>TLSI_0008_OPTION2</t>
-  </si>
-  <si>
-    <t>TLSI_0003_OPTION1</t>
-  </si>
-  <si>
-    <t>TLSI_0003_OPTION2</t>
-  </si>
-  <si>
     <t>Wie gerne lesen oder hören (z.B. Audiobuch) Sie Lyrik (alle Arten von Gedichten, Dichtung)?</t>
   </si>
   <si>
@@ -299,6 +185,120 @@
   </si>
   <si>
     <t>Fragebogen Literarische Interessen</t>
+  </si>
+  <si>
+    <t>TLIQ_0000_PROMPT</t>
+  </si>
+  <si>
+    <t>TLIQ_0001_PROMPT</t>
+  </si>
+  <si>
+    <t>TLIQ_0002_PROMPT</t>
+  </si>
+  <si>
+    <t>TLIQ_0003_PROMPT</t>
+  </si>
+  <si>
+    <t>TLIQ_0003_OPTION1</t>
+  </si>
+  <si>
+    <t>TLIQ_0003_OPTION2</t>
+  </si>
+  <si>
+    <t>TLIQ_0003_CHOICE1</t>
+  </si>
+  <si>
+    <t>TLIQ_0003_CHOICE2</t>
+  </si>
+  <si>
+    <t>TLIQ_0003_CHOICE3</t>
+  </si>
+  <si>
+    <t>TLIQ_0003_CHOICE4</t>
+  </si>
+  <si>
+    <t>TLIQ_0003_CHOICE5</t>
+  </si>
+  <si>
+    <t>TLIQ_0003_CHOICE6</t>
+  </si>
+  <si>
+    <t>TLIQ_0003_CHOICE7</t>
+  </si>
+  <si>
+    <t>TLIQ_0004_PROMPT</t>
+  </si>
+  <si>
+    <t>TLIQ_0004_CHOICE1</t>
+  </si>
+  <si>
+    <t>TLIQ_0004_CHOICE2</t>
+  </si>
+  <si>
+    <t>TLIQ_0005_PROMPT</t>
+  </si>
+  <si>
+    <t>TLIQ_0005_UNIT</t>
+  </si>
+  <si>
+    <t>TLIQ_0005_OPTION1</t>
+  </si>
+  <si>
+    <t>TLIQ_0005_OPTION2</t>
+  </si>
+  <si>
+    <t>TLIQ_0005_OPTION3</t>
+  </si>
+  <si>
+    <t>TLIQ_0005_OPTION4</t>
+  </si>
+  <si>
+    <t>TLIQ_0005_OPTION5</t>
+  </si>
+  <si>
+    <t>TLIQ_0006_PROMPT</t>
+  </si>
+  <si>
+    <t>TLIQ_0006_UNIT</t>
+  </si>
+  <si>
+    <t>TLIQ_0006_OPTION1</t>
+  </si>
+  <si>
+    <t>TLIQ_0006_OPTION2</t>
+  </si>
+  <si>
+    <t>TLIQ_0006_OPTION3</t>
+  </si>
+  <si>
+    <t>TLIQ_0006_OPTION4</t>
+  </si>
+  <si>
+    <t>TLIQ_0006_OPTION5</t>
+  </si>
+  <si>
+    <t>TLIQ_0007_PROMPT</t>
+  </si>
+  <si>
+    <t>TLIQ_0007_UNIT</t>
+  </si>
+  <si>
+    <t>TLIQ_0007_OPTION1</t>
+  </si>
+  <si>
+    <t>TLIQ_0007_OPTION2</t>
+  </si>
+  <si>
+    <t>TLIQ_0008_PROMPT</t>
+  </si>
+  <si>
+    <t>TLIQ_0008_UNIT</t>
+  </si>
+  <si>
+    <t>TLIQ_0008_OPTION1</t>
+  </si>
+  <si>
+    <t>TLIQ_0008_OPTION2</t>
   </si>
 </sst>
 </file>
@@ -1208,420 +1208,420 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Tones of small changes, added Drama to LIQ, added de_f
</commit_message>
<xml_diff>
--- a/data_raw/dicts/LIQ_dict.xlsx
+++ b/data_raw/dicts/LIQ_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E40A5C-59E3-4F3D-B31D-071DC2C4EFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0C2063-918C-456F-9BCF-8D8AAF6158D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LIQ_dict" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="102">
   <si>
     <t>key</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Haben Sie schon einmal einen Kurs in kreativem Schreiben belegt?</t>
   </si>
   <si>
-    <t>Bitte schätzen Sie ein, wie viele Stunden Sie durchschnittlich in einer typischen Woche die folgenden Arten von Texten lesen.</t>
-  </si>
-  <si>
     <t>Nachrichten (z.B. Zeitungen, Zeitschriften, Internetmaterial)</t>
   </si>
   <si>
@@ -127,15 +124,6 @@
     <t>Poetry (all types of poems, poetry)</t>
   </si>
   <si>
-    <t>Denken Sie nun bitte einmal an die Zeit in Ihrem Leben, als Sie sich am meisten mit Literatur beschäftigt haben. \\ Wie viele Stunden haben Sie auf dem Höhepunkt Ihres literarischen Interesses durchschnittlich in einer Woche damit verbracht, die folgenden literarischen Gattungen zu lesen.</t>
-  </si>
-  <si>
-    <t>Wie gerne lesen oder hören (z.B. Audiobuch) Sie Lyrik (alle Arten von Gedichten, Dichtung)?</t>
-  </si>
-  <si>
-    <t>Wie gerne lesen oder hören (z.B. Audiobuch) Sie Prosa (z.B. Romane, Erzählungen, Kurzgeschichten)?</t>
-  </si>
-  <si>
     <t>How much do you like reading or listening (e.g. audio book) to</t>
   </si>
   <si>
@@ -163,12 +151,6 @@
     <t>Have you ever taken a creative writing course?</t>
   </si>
   <si>
-    <t>Please estimate how many hours on average you read the following types of texts in a typical week.</t>
-  </si>
-  <si>
-    <t>Now please think about the time in your life when you were most involved with literature. \\ At the peak of your literary interest, how many hours did you spend on average in a week reading the following literary genres?</t>
-  </si>
-  <si>
     <t>Please estimate how many hours on average you spend **writing** the following types of texts in a typical week.</t>
   </si>
   <si>
@@ -299,6 +281,51 @@
   </si>
   <si>
     <t>TLIQ_0008_OPTION2</t>
+  </si>
+  <si>
+    <t>TLIQ_0003_OPTION3</t>
+  </si>
+  <si>
+    <t>How much do you like reading or listening (e.g. audio book) to plays (e.g., comedies, tragedies)?</t>
+  </si>
+  <si>
+    <t>TLIQ_0006_OPTION6</t>
+  </si>
+  <si>
+    <t>Dramen (z.B. Komödien, Tragödien)</t>
+  </si>
+  <si>
+    <t>Plays (e.g., comedies, tragedies)</t>
+  </si>
+  <si>
+    <t>TLIQ_0008_OPTION3</t>
+  </si>
+  <si>
+    <t>TLIQ_0007_OPTION3</t>
+  </si>
+  <si>
+    <t>TLIQ_0005_OPTION6</t>
+  </si>
+  <si>
+    <t>Wie gerne lesen oder hören (z.B. Audiobuch) Sie **Prosa** (z.B. Romane, Erzählungen, Kurzgeschichten)?</t>
+  </si>
+  <si>
+    <t>Wie gerne lesen oder hören (z.B. Audiobuch) Sie **Lyrik** (alle Arten von Gedichten, Dichtung)?</t>
+  </si>
+  <si>
+    <t>Wie gerne lesen oder hören (z.B. Audiobuch) Sie **Dramen** (z.B. Komödien, Tragödien)?</t>
+  </si>
+  <si>
+    <t>Bitte schätzen Sie ein, wie viele Stunden Sie durchschnittlich in einer typischen Woche die folgenden Arten von Texten **lesen**.</t>
+  </si>
+  <si>
+    <t>Please estimate how many hours on average you **read** the following types of texts in a typical week.</t>
+  </si>
+  <si>
+    <t>Denken Sie nun bitte einmal an die Zeit in Ihrem Leben, als Sie sich am meisten mit Literatur beschäftigt haben. \\ Wie viele Stunden haben Sie auf dem Höhepunkt Ihres literarischen Interesses durchschnittlich in einer Woche damit verbracht, die folgenden literarischen Gattungen zu **lesen**.</t>
+  </si>
+  <si>
+    <t>Now please think about the time in your life when you were most involved with literature. \\ At the peak of your literary interest, how many hours did you spend on average in a week **reading** the following literary genres?</t>
   </si>
 </sst>
 </file>
@@ -1182,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,131 +1235,131 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>87</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>55</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>41</v>
@@ -1340,306 +1367,361 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="3" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="3" t="s">
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="4" t="s">
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B33" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B34" s="3" t="s">
+    </row>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" s="3" t="s">
+      <c r="C37" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="1"/>
-    </row>
-    <row r="59" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="1"/>
-    </row>
-    <row r="65" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="66" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C66" s="1"/>
-    </row>
-    <row r="71" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="B44" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="1"/>
+    </row>
+    <row r="63" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="69" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="1"/>
+    </row>
+    <row r="75" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>